<commit_message>
changed index time_series..._city to gemeente_id
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
   <si>
     <t>Provincienaam</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>08-03-2020</t>
+  </si>
+  <si>
+    <t>gemeente_id</t>
   </si>
   <si>
     <t>Zuid-Holland</t>
@@ -717,6 +720,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,10 +768,10 @@
         <v>518</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -806,10 +812,10 @@
         <v>796</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -850,10 +856,10 @@
         <v>613</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -894,10 +900,10 @@
         <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -938,10 +944,10 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -982,10 +988,10 @@
         <v>484</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1026,10 +1032,10 @@
         <v>1959</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1070,10 +1076,10 @@
         <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1114,10 +1120,10 @@
         <v>363</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1158,10 +1164,10 @@
         <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1202,10 +1208,10 @@
         <v>1954</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1246,10 +1252,10 @@
         <v>748</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1290,10 +1296,10 @@
         <v>1721</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1334,10 +1340,10 @@
         <v>753</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1378,10 +1384,10 @@
         <v>209</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1422,10 +1428,10 @@
         <v>375</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1466,10 +1472,10 @@
         <v>376</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1510,10 +1516,10 @@
         <v>377</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1554,10 +1560,10 @@
         <v>755</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1598,10 +1604,10 @@
         <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1642,10 +1648,10 @@
         <v>758</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1686,10 +1692,10 @@
         <v>1876</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1730,10 +1736,10 @@
         <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1774,10 +1780,10 @@
         <v>216</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1818,10 +1824,10 @@
         <v>310</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1862,10 +1868,10 @@
         <v>503</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1906,10 +1912,10 @@
         <v>762</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1950,10 +1956,10 @@
         <v>384</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1994,10 +2000,10 @@
         <v>1774</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2038,10 +2044,10 @@
         <v>766</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2082,10 +2088,10 @@
         <v>772</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2126,10 +2132,10 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2170,10 +2176,10 @@
         <v>1652</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2214,10 +2220,10 @@
         <v>785</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2258,10 +2264,10 @@
         <v>1942</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2302,10 +2308,10 @@
         <v>512</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2346,10 +2352,10 @@
         <v>392</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2390,10 +2396,10 @@
         <v>523</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2434,10 +2440,10 @@
         <v>397</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2478,10 +2484,10 @@
         <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2522,10 +2528,10 @@
         <v>794</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2566,10 +2572,10 @@
         <v>797</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2610,10 +2616,10 @@
         <v>1963</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2654,10 +2660,10 @@
         <v>321</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2698,10 +2704,10 @@
         <v>406</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2742,10 +2748,10 @@
         <v>353</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2786,10 +2792,10 @@
         <v>1931</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2830,10 +2836,10 @@
         <v>1685</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2874,10 +2880,10 @@
         <v>415</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2918,10 +2924,10 @@
         <v>1621</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2962,10 +2968,10 @@
         <v>1916</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -3006,10 +3012,10 @@
         <v>1705</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3050,10 +3056,10 @@
         <v>809</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -3094,10 +3100,10 @@
         <v>263</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -3138,10 +3144,10 @@
         <v>935</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -3182,10 +3188,10 @@
         <v>1948</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3226,10 +3232,10 @@
         <v>268</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3270,10 +3276,10 @@
         <v>579</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3314,10 +3320,10 @@
         <v>824</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -3358,10 +3364,10 @@
         <v>828</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3402,10 +3408,10 @@
         <v>1926</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3446,10 +3452,10 @@
         <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3490,10 +3496,10 @@
         <v>597</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3534,10 +3540,10 @@
         <v>957</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3578,10 +3584,10 @@
         <v>599</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3622,10 +3628,10 @@
         <v>1676</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3666,10 +3672,10 @@
         <v>965</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3710,10 +3716,10 @@
         <v>845</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3754,10 +3760,10 @@
         <v>1883</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -3798,10 +3804,10 @@
         <v>342</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3842,10 +3848,10 @@
         <v>1904</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3886,10 +3892,10 @@
         <v>855</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3930,10 +3936,10 @@
         <v>856</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3974,10 +3980,10 @@
         <v>344</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -4018,10 +4024,10 @@
         <v>1581</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -4062,10 +4068,10 @@
         <v>1961</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -4106,10 +4112,10 @@
         <v>866</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C78" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -4150,10 +4156,10 @@
         <v>867</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -4194,10 +4200,10 @@
         <v>852</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -4238,10 +4244,10 @@
         <v>1960</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -4282,10 +4288,10 @@
         <v>668</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -4326,10 +4332,10 @@
         <v>614</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -4370,10 +4376,10 @@
         <v>296</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C84" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -4414,10 +4420,10 @@
         <v>352</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -4458,10 +4464,10 @@
         <v>632</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -4502,10 +4508,10 @@
         <v>479</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -4546,10 +4552,10 @@
         <v>297</v>
       </c>
       <c r="B88" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -4590,10 +4596,10 @@
         <v>50</v>
       </c>
       <c r="B89" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -4634,10 +4640,10 @@
         <v>355</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -4678,10 +4684,10 @@
         <v>879</v>
       </c>
       <c r="B91" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -4722,10 +4728,10 @@
         <v>193</v>
       </c>
       <c r="B92" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C92" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D92">
         <v>0</v>

</xml_diff>

<commit_message>
changed main.py to use cronjobs
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="155">
   <si>
     <t>Provincienaam</t>
   </si>
@@ -437,6 +437,48 @@
   </si>
   <si>
     <t>Zwolle</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>27.0</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>29.0</t>
+  </si>
+  <si>
+    <t>14.0</t>
   </si>
 </sst>
 </file>
@@ -896,8 +938,8 @@
       <c r="O2">
         <v>2</v>
       </c>
-      <c r="P2">
-        <v>3</v>
+      <c r="P2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -946,8 +988,8 @@
       <c r="O3">
         <v>3</v>
       </c>
-      <c r="P3">
-        <v>4</v>
+      <c r="P3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -996,8 +1038,8 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
-        <v>2</v>
+      <c r="P4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1046,8 +1088,8 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>1</v>
+      <c r="P5" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1096,8 +1138,8 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>1</v>
+      <c r="P6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1146,8 +1188,8 @@
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7">
-        <v>1</v>
+      <c r="P7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1196,8 +1238,8 @@
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8">
-        <v>1</v>
+      <c r="P8" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1246,8 +1288,8 @@
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9">
-        <v>1</v>
+      <c r="P9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1296,8 +1338,8 @@
       <c r="O10">
         <v>4</v>
       </c>
-      <c r="P10">
-        <v>4</v>
+      <c r="P10" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1346,8 +1388,8 @@
       <c r="O11">
         <v>2</v>
       </c>
-      <c r="P11">
-        <v>2</v>
+      <c r="P11" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1396,8 +1438,8 @@
       <c r="O12">
         <v>4</v>
       </c>
-      <c r="P12">
-        <v>8</v>
+      <c r="P12" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1446,8 +1488,8 @@
       <c r="O13">
         <v>2</v>
       </c>
-      <c r="P13">
-        <v>2</v>
+      <c r="P13" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1496,8 +1538,8 @@
       <c r="O14">
         <v>4</v>
       </c>
-      <c r="P14">
-        <v>5</v>
+      <c r="P14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1546,8 +1588,8 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
-        <v>1</v>
+      <c r="P15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1596,8 +1638,8 @@
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>1</v>
+      <c r="P16" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1646,8 +1688,8 @@
       <c r="O17">
         <v>2</v>
       </c>
-      <c r="P17">
-        <v>2</v>
+      <c r="P17" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1696,8 +1738,8 @@
       <c r="O18">
         <v>2</v>
       </c>
-      <c r="P18">
-        <v>2</v>
+      <c r="P18" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1746,8 +1788,8 @@
       <c r="O19">
         <v>3</v>
       </c>
-      <c r="P19">
-        <v>3</v>
+      <c r="P19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1796,8 +1838,8 @@
       <c r="O20">
         <v>4</v>
       </c>
-      <c r="P20">
-        <v>4</v>
+      <c r="P20" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1846,8 +1888,8 @@
       <c r="O21">
         <v>1</v>
       </c>
-      <c r="P21">
-        <v>1</v>
+      <c r="P21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1896,8 +1938,8 @@
       <c r="O22">
         <v>1</v>
       </c>
-      <c r="P22">
-        <v>1</v>
+      <c r="P22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1946,8 +1988,8 @@
       <c r="O23">
         <v>1</v>
       </c>
-      <c r="P23">
-        <v>2</v>
+      <c r="P23" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1996,8 +2038,8 @@
       <c r="O24">
         <v>3</v>
       </c>
-      <c r="P24">
-        <v>3</v>
+      <c r="P24" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2046,8 +2088,8 @@
       <c r="O25">
         <v>19</v>
       </c>
-      <c r="P25">
-        <v>27</v>
+      <c r="P25" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2096,8 +2138,8 @@
       <c r="O26">
         <v>2</v>
       </c>
-      <c r="P26">
-        <v>2</v>
+      <c r="P26" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2146,8 +2188,8 @@
       <c r="O27">
         <v>9</v>
       </c>
-      <c r="P27">
-        <v>11</v>
+      <c r="P27" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2196,8 +2238,8 @@
       <c r="O28">
         <v>1</v>
       </c>
-      <c r="P28">
-        <v>1</v>
+      <c r="P28" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2246,8 +2288,8 @@
       <c r="O29">
         <v>6</v>
       </c>
-      <c r="P29">
-        <v>6</v>
+      <c r="P29" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2296,8 +2338,8 @@
       <c r="O30">
         <v>1</v>
       </c>
-      <c r="P30">
-        <v>1</v>
+      <c r="P30" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2346,8 +2388,8 @@
       <c r="O31">
         <v>1</v>
       </c>
-      <c r="P31">
-        <v>1</v>
+      <c r="P31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2396,8 +2438,8 @@
       <c r="O32">
         <v>2</v>
       </c>
-      <c r="P32">
-        <v>2</v>
+      <c r="P32" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2446,8 +2488,8 @@
       <c r="O33">
         <v>2</v>
       </c>
-      <c r="P33">
-        <v>2</v>
+      <c r="P33" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2496,8 +2538,8 @@
       <c r="O34">
         <v>3</v>
       </c>
-      <c r="P34">
-        <v>3</v>
+      <c r="P34" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2546,8 +2588,8 @@
       <c r="O35">
         <v>7</v>
       </c>
-      <c r="P35">
-        <v>8</v>
+      <c r="P35" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2596,8 +2638,8 @@
       <c r="O36">
         <v>1</v>
       </c>
-      <c r="P36">
-        <v>1</v>
+      <c r="P36" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -2646,8 +2688,8 @@
       <c r="O37">
         <v>0</v>
       </c>
-      <c r="P37">
-        <v>1</v>
+      <c r="P37" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2696,8 +2738,8 @@
       <c r="O38">
         <v>1</v>
       </c>
-      <c r="P38">
-        <v>3</v>
+      <c r="P38" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2746,8 +2788,8 @@
       <c r="O39">
         <v>1</v>
       </c>
-      <c r="P39">
-        <v>2</v>
+      <c r="P39" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2796,8 +2838,8 @@
       <c r="O40">
         <v>0</v>
       </c>
-      <c r="P40">
-        <v>1</v>
+      <c r="P40" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -2846,8 +2888,8 @@
       <c r="O41">
         <v>4</v>
       </c>
-      <c r="P41">
-        <v>4</v>
+      <c r="P41" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -2896,8 +2938,8 @@
       <c r="O42">
         <v>2</v>
       </c>
-      <c r="P42">
-        <v>2</v>
+      <c r="P42" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -2996,8 +3038,8 @@
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="P44">
-        <v>1</v>
+      <c r="P44" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3046,8 +3088,8 @@
       <c r="O45">
         <v>2</v>
       </c>
-      <c r="P45">
-        <v>2</v>
+      <c r="P45" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3096,8 +3138,8 @@
       <c r="O46">
         <v>2</v>
       </c>
-      <c r="P46">
-        <v>1</v>
+      <c r="P46" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3146,8 +3188,8 @@
       <c r="O47">
         <v>4</v>
       </c>
-      <c r="P47">
-        <v>5</v>
+      <c r="P47" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3196,8 +3238,8 @@
       <c r="O48">
         <v>1</v>
       </c>
-      <c r="P48">
-        <v>1</v>
+      <c r="P48" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3246,8 +3288,8 @@
       <c r="O49">
         <v>2</v>
       </c>
-      <c r="P49">
-        <v>2</v>
+      <c r="P49" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3296,8 +3338,8 @@
       <c r="O50">
         <v>7</v>
       </c>
-      <c r="P50">
-        <v>11</v>
+      <c r="P50" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3346,8 +3388,8 @@
       <c r="O51">
         <v>1</v>
       </c>
-      <c r="P51">
-        <v>1</v>
+      <c r="P51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -3396,8 +3438,8 @@
       <c r="O52">
         <v>2</v>
       </c>
-      <c r="P52">
-        <v>2</v>
+      <c r="P52" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3446,8 +3488,8 @@
       <c r="O53">
         <v>13</v>
       </c>
-      <c r="P53">
-        <v>13</v>
+      <c r="P53" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -3496,8 +3538,8 @@
       <c r="O54">
         <v>1</v>
       </c>
-      <c r="P54">
-        <v>1</v>
+      <c r="P54" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -3546,8 +3588,8 @@
       <c r="O55">
         <v>1</v>
       </c>
-      <c r="P55">
-        <v>1</v>
+      <c r="P55" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -3596,8 +3638,8 @@
       <c r="O56">
         <v>1</v>
       </c>
-      <c r="P56">
-        <v>1</v>
+      <c r="P56" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3646,8 +3688,8 @@
       <c r="O57">
         <v>2</v>
       </c>
-      <c r="P57">
-        <v>1</v>
+      <c r="P57" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -3746,8 +3788,8 @@
       <c r="O59">
         <v>3</v>
       </c>
-      <c r="P59">
-        <v>4</v>
+      <c r="P59" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -3796,8 +3838,8 @@
       <c r="O60">
         <v>0</v>
       </c>
-      <c r="P60">
-        <v>1</v>
+      <c r="P60" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -3846,8 +3888,8 @@
       <c r="O61">
         <v>1</v>
       </c>
-      <c r="P61">
-        <v>2</v>
+      <c r="P61" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -3896,8 +3938,8 @@
       <c r="O62">
         <v>1</v>
       </c>
-      <c r="P62">
-        <v>2</v>
+      <c r="P62" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -3946,8 +3988,8 @@
       <c r="O63">
         <v>2</v>
       </c>
-      <c r="P63">
-        <v>2</v>
+      <c r="P63" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -3996,8 +4038,8 @@
       <c r="O64">
         <v>7</v>
       </c>
-      <c r="P64">
-        <v>7</v>
+      <c r="P64" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -4046,8 +4088,8 @@
       <c r="O65">
         <v>1</v>
       </c>
-      <c r="P65">
-        <v>1</v>
+      <c r="P65" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -4096,8 +4138,8 @@
       <c r="O66">
         <v>6</v>
       </c>
-      <c r="P66">
-        <v>7</v>
+      <c r="P66" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -4146,8 +4188,8 @@
       <c r="O67">
         <v>10</v>
       </c>
-      <c r="P67">
-        <v>11</v>
+      <c r="P67" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -4196,8 +4238,8 @@
       <c r="O68">
         <v>1</v>
       </c>
-      <c r="P68">
-        <v>1</v>
+      <c r="P68" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:16">
@@ -4246,8 +4288,8 @@
       <c r="O69">
         <v>3</v>
       </c>
-      <c r="P69">
-        <v>3</v>
+      <c r="P69" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -4296,8 +4338,8 @@
       <c r="O70">
         <v>2</v>
       </c>
-      <c r="P70">
-        <v>2</v>
+      <c r="P70" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:16">
@@ -4346,8 +4388,8 @@
       <c r="O71">
         <v>0</v>
       </c>
-      <c r="P71">
-        <v>1</v>
+      <c r="P71" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -4396,8 +4438,8 @@
       <c r="O72">
         <v>1</v>
       </c>
-      <c r="P72">
-        <v>1</v>
+      <c r="P72" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:16">
@@ -4446,8 +4488,8 @@
       <c r="O73">
         <v>3</v>
       </c>
-      <c r="P73">
-        <v>3</v>
+      <c r="P73" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -4496,8 +4538,8 @@
       <c r="O74">
         <v>0</v>
       </c>
-      <c r="P74">
-        <v>2</v>
+      <c r="P74" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -4546,8 +4588,8 @@
       <c r="O75">
         <v>1</v>
       </c>
-      <c r="P75">
-        <v>1</v>
+      <c r="P75" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -4596,8 +4638,8 @@
       <c r="O76">
         <v>0</v>
       </c>
-      <c r="P76">
-        <v>1</v>
+      <c r="P76" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -4646,8 +4688,8 @@
       <c r="O77">
         <v>2</v>
       </c>
-      <c r="P77">
-        <v>4</v>
+      <c r="P77" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -4696,8 +4738,8 @@
       <c r="O78">
         <v>5</v>
       </c>
-      <c r="P78">
-        <v>5</v>
+      <c r="P78" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -4746,8 +4788,8 @@
       <c r="O79">
         <v>0</v>
       </c>
-      <c r="P79">
-        <v>1</v>
+      <c r="P79" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -4796,8 +4838,8 @@
       <c r="O80">
         <v>1</v>
       </c>
-      <c r="P80">
-        <v>1</v>
+      <c r="P80" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -4846,8 +4888,8 @@
       <c r="O81">
         <v>1</v>
       </c>
-      <c r="P81">
-        <v>1</v>
+      <c r="P81" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -4896,8 +4938,8 @@
       <c r="O82">
         <v>14</v>
       </c>
-      <c r="P82">
-        <v>15</v>
+      <c r="P82" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -4946,8 +4988,8 @@
       <c r="O83">
         <v>0</v>
       </c>
-      <c r="P83">
-        <v>1</v>
+      <c r="P83" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -4996,8 +5038,8 @@
       <c r="O84">
         <v>1</v>
       </c>
-      <c r="P84">
-        <v>2</v>
+      <c r="P84" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -5046,8 +5088,8 @@
       <c r="O85">
         <v>2</v>
       </c>
-      <c r="P85">
-        <v>2</v>
+      <c r="P85" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -5096,8 +5138,8 @@
       <c r="O86">
         <v>5</v>
       </c>
-      <c r="P86">
-        <v>5</v>
+      <c r="P86" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -5146,8 +5188,8 @@
       <c r="O87">
         <v>8</v>
       </c>
-      <c r="P87">
-        <v>13</v>
+      <c r="P87" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -5196,8 +5238,8 @@
       <c r="O88">
         <v>7</v>
       </c>
-      <c r="P88">
-        <v>8</v>
+      <c r="P88" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -5246,8 +5288,8 @@
       <c r="O89">
         <v>5</v>
       </c>
-      <c r="P89">
-        <v>5</v>
+      <c r="P89" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -5296,8 +5338,8 @@
       <c r="O90">
         <v>1</v>
       </c>
-      <c r="P90">
-        <v>1</v>
+      <c r="P90" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -5346,8 +5388,8 @@
       <c r="O91">
         <v>27</v>
       </c>
-      <c r="P91">
-        <v>29</v>
+      <c r="P91" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -5396,8 +5438,8 @@
       <c r="O92">
         <v>1</v>
       </c>
-      <c r="P92">
-        <v>1</v>
+      <c r="P92" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -5446,8 +5488,8 @@
       <c r="O93">
         <v>12</v>
       </c>
-      <c r="P93">
-        <v>13</v>
+      <c r="P93" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -5496,8 +5538,8 @@
       <c r="O94">
         <v>13</v>
       </c>
-      <c r="P94">
-        <v>14</v>
+      <c r="P94" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -5546,8 +5588,8 @@
       <c r="O95">
         <v>2</v>
       </c>
-      <c r="P95">
-        <v>2</v>
+      <c r="P95" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:16">
@@ -5596,8 +5638,8 @@
       <c r="O96">
         <v>1</v>
       </c>
-      <c r="P96">
-        <v>1</v>
+      <c r="P96" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:16">
@@ -5646,8 +5688,8 @@
       <c r="O97">
         <v>1</v>
       </c>
-      <c r="P97">
-        <v>1</v>
+      <c r="P97" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:16">
@@ -5696,8 +5738,8 @@
       <c r="O98">
         <v>1</v>
       </c>
-      <c r="P98">
-        <v>1</v>
+      <c r="P98" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:16">
@@ -5746,8 +5788,8 @@
       <c r="O99">
         <v>1</v>
       </c>
-      <c r="P99">
-        <v>1</v>
+      <c r="P99" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:16">
@@ -5796,8 +5838,8 @@
       <c r="O100">
         <v>1</v>
       </c>
-      <c r="P100">
-        <v>1</v>
+      <c r="P100" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -5846,8 +5888,8 @@
       <c r="O101">
         <v>1</v>
       </c>
-      <c r="P101">
-        <v>1</v>
+      <c r="P101" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -5896,8 +5938,8 @@
       <c r="O102">
         <v>5</v>
       </c>
-      <c r="P102">
-        <v>5</v>
+      <c r="P102" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:16">
@@ -5946,8 +5988,8 @@
       <c r="O103">
         <v>0</v>
       </c>
-      <c r="P103">
-        <v>1</v>
+      <c r="P103" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -5996,8 +6038,8 @@
       <c r="O104">
         <v>1</v>
       </c>
-      <c r="P104">
-        <v>1</v>
+      <c r="P104" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:16">
@@ -6046,8 +6088,8 @@
       <c r="O105">
         <v>2</v>
       </c>
-      <c r="P105">
-        <v>2</v>
+      <c r="P105" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:16">
@@ -6096,8 +6138,8 @@
       <c r="O106">
         <v>1</v>
       </c>
-      <c r="P106">
-        <v>1</v>
+      <c r="P106" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:16">
@@ -6146,8 +6188,8 @@
       <c r="O107">
         <v>1</v>
       </c>
-      <c r="P107">
-        <v>1</v>
+      <c r="P107" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:16">
@@ -6196,8 +6238,8 @@
       <c r="O108">
         <v>1</v>
       </c>
-      <c r="P108">
-        <v>1</v>
+      <c r="P108" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:16">
@@ -6246,8 +6288,8 @@
       <c r="O109">
         <v>1</v>
       </c>
-      <c r="P109">
-        <v>1</v>
+      <c r="P109" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:16">
@@ -6296,8 +6338,8 @@
       <c r="O110">
         <v>2</v>
       </c>
-      <c r="P110">
-        <v>2</v>
+      <c r="P110" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -6346,8 +6388,8 @@
       <c r="O111">
         <v>2</v>
       </c>
-      <c r="P111">
-        <v>2</v>
+      <c r="P111" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:16">
@@ -6396,8 +6438,8 @@
       <c r="O112">
         <v>1</v>
       </c>
-      <c r="P112">
-        <v>1</v>
+      <c r="P112" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -6446,8 +6488,8 @@
       <c r="O113">
         <v>1</v>
       </c>
-      <c r="P113">
-        <v>1</v>
+      <c r="P113" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -6496,8 +6538,8 @@
       <c r="O114">
         <v>1</v>
       </c>
-      <c r="P114">
-        <v>2</v>
+      <c r="P114" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -6546,8 +6588,8 @@
       <c r="O115">
         <v>1</v>
       </c>
-      <c r="P115">
-        <v>1</v>
+      <c r="P115" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:16">
@@ -6596,8 +6638,8 @@
       <c r="O116">
         <v>1</v>
       </c>
-      <c r="P116">
-        <v>1</v>
+      <c r="P116" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 20200311 RIVM rectification
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
@@ -16195,7 +16195,7 @@
         <v>2</v>
       </c>
       <c r="R262">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:18">
@@ -18491,7 +18491,7 @@
         <v>0</v>
       </c>
       <c r="R303">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="304" spans="1:18">

</xml_diff>